<commit_message>
close #5 joining is now working
</commit_message>
<xml_diff>
--- a/test/data/test_join1.xlsx
+++ b/test/data/test_join1.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">ID</t>
+    <t xml:space="preserve">Idé</t>
   </si>
   <si>
     <t xml:space="preserve">Nom</t>
@@ -160,17 +160,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A3:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -245,8 +245,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>